<commit_message>
Enhance SCT processing logic to support file downloads and improve output handling
</commit_message>
<xml_diff>
--- a/ejemplos_api/sct.xlsx
+++ b/ejemplos_api/sct.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,36 @@
           <t>presentacion_ddjj</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ubicacion_deuda</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>nombre_deuda</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ubicacion_vencimientos</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>nombre_vencimientos</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ubicacion_ddjj</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>nombre_ddjj</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -506,6 +536,36 @@
           <t>SI</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>./Descargas</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>deuda-demo</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>./Descargas</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>vencimientos-demo</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>./Descargas</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ddjj-demo</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,6 +601,36 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>NO</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>./Descargas</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>deuda-no</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>./Descargas</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>vencimientos-no</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>./Descargas</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>ddjj-no</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update SCT Excel file to reflect recent changes in data structure
</commit_message>
<xml_diff>
--- a/ejemplos_api/sct.xlsx
+++ b/ejemplos_api/sct.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,30 +471,45 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>excel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>csv</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>ubicacion_deuda</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>nombre_deuda</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>ubicacion_vencimientos</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>nombre_vencimientos</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>ubicacion_ddjj</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>nombre_ddjj</t>
         </is>
@@ -538,30 +553,45 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>./Descargas</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>deuda-demo</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>./Descargas</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>vencimientos-demo</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>./Descargas</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>ddjj-demo</t>
         </is>
@@ -605,30 +635,45 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>./Descargas</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>deuda-no</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>./Descargas</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>vencimientos-no</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>./Descargas</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>ddjj-no</t>
         </is>

</xml_diff>